<commit_message>
Validated EPV component (erythyro)
</commit_message>
<xml_diff>
--- a/tabular/eve/epv-erythyro-side-data.xlsx
+++ b/tabular/eve/epv-erythyro-side-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rob/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertgifford/Projects/virus/comparative/DNAss/Parvoviridae-GLUE/tabular/eve/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D7C47C8-2E70-9C44-9363-3A0C115DC5A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E171C47-F0B7-AD46-A177-36B5501563B0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1340" yWindow="8520" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="21400" yWindow="7880" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="query_result" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
   <si>
     <t>host_species</t>
   </si>
@@ -139,9 +139,6 @@
     <t>PVJX010011861.1</t>
   </si>
   <si>
-    <t>erythryo.2-Dolichotis_patagonum</t>
-  </si>
-  <si>
     <t>Indri_indri</t>
   </si>
   <si>
@@ -163,9 +160,6 @@
     <t>RJWJ010000280.1</t>
   </si>
   <si>
-    <t>erythryo.1-indri</t>
-  </si>
-  <si>
     <t>sequenceID</t>
   </si>
   <si>
@@ -181,13 +175,19 @@
     <t>erythyro.1-Indri_indri</t>
   </si>
   <si>
-    <t>erythryo.2</t>
-  </si>
-  <si>
-    <t>erythryo.1</t>
-  </si>
-  <si>
-    <t>erythryo.2-dolichotis</t>
+    <t>erythyro.2-Dolichotis_patagonum</t>
+  </si>
+  <si>
+    <t>erythyro.2-dolichotis</t>
+  </si>
+  <si>
+    <t>erythyro.1-indri</t>
+  </si>
+  <si>
+    <t>erythyro.1</t>
+  </si>
+  <si>
+    <t>erythyro.2</t>
   </si>
 </sst>
 </file>
@@ -1046,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B3" sqref="A1:AE3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1063,19 +1063,19 @@
   <sheetData>
     <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>49</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>6</v>
@@ -1157,20 +1157,20 @@
       </c>
     </row>
     <row r="2" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
-        <v>10</v>
+      <c r="A2" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D2" s="3">
         <v>2</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>31</v>
@@ -1252,14 +1252,14 @@
       </c>
     </row>
     <row r="3" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
-        <v>175</v>
+      <c r="A3" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -1268,19 +1268,19 @@
         <v>54</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>28</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>29</v>
@@ -1337,13 +1337,13 @@
         <v>32</v>
       </c>
       <c r="AC3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AD3" s="3" t="s">
+      <c r="AE3" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="AE3" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>